<commit_message>
adding invoice generation + dashboard analysis
</commit_message>
<xml_diff>
--- a/backend/Invoice Template.xlsx
+++ b/backend/Invoice Template.xlsx
@@ -121,7 +121,7 @@
     <t>UNIT PRICE</t>
   </si>
   <si>
-    <t>SUBTOTAL</t>
+    <t>SUBTOTAL (SGD)</t>
   </si>
   <si>
     <t>Total</t>
@@ -1724,8 +1724,8 @@
   </sheetPr>
   <dimension ref="B1:K46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="60" showRuler="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="60" showRuler="0" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
Adding the MYR into the currency selection
</commit_message>
<xml_diff>
--- a/backend/Invoice Template.xlsx
+++ b/backend/Invoice Template.xlsx
@@ -118,10 +118,10 @@
     <t>QTY</t>
   </si>
   <si>
-    <t>UNIT PRICE (SGD)</t>
-  </si>
-  <si>
-    <t>SUBTOTAL (SGD)</t>
+    <t xml:space="preserve">UNIT PRICE </t>
+  </si>
+  <si>
+    <t>SUBTOTAL</t>
   </si>
   <si>
     <t>Total</t>
@@ -1711,7 +1711,7 @@
   </sheetPr>
   <dimension ref="B1:K46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="60" showRuler="0" topLeftCell="A14" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="60" showRuler="0" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding target currency logic
</commit_message>
<xml_diff>
--- a/backend/Invoice Template.xlsx
+++ b/backend/Invoice Template.xlsx
@@ -1711,8 +1711,8 @@
   </sheetPr>
   <dimension ref="B1:K46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="60" showRuler="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="60" showRuler="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" customHeight="1"/>

</xml_diff>